<commit_message>
clothes-shop database design 09.04.2022
</commit_message>
<xml_diff>
--- a/Database Design.xlsx
+++ b/Database Design.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94BA3BE2-B3B6-4E6A-8BC0-07AB82F9D4C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04B9EC11-F96F-4E67-B666-FBCFF70B9F13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3075" yWindow="1905" windowWidth="21600" windowHeight="11385" tabRatio="749" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="749" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Mô hình quan niệm" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="165">
   <si>
     <t>1. Xác định các đối tượng và thông tin cần lưu trữ</t>
   </si>
@@ -477,9 +477,6 @@
     <t>TenKT</t>
   </si>
   <si>
-    <t>GhiChu</t>
-  </si>
-  <si>
     <t>MaMS</t>
   </si>
   <si>
@@ -489,50 +486,44 @@
     <t>TenMau</t>
   </si>
   <si>
-    <t>TenChatLieu</t>
-  </si>
-  <si>
-    <t>ChiTietKichThuoc</t>
-  </si>
-  <si>
-    <t>ChiTietMauSac</t>
-  </si>
-  <si>
     <t>HinhAnh</t>
   </si>
   <si>
-    <t>ChiTietChatLieu</t>
-  </si>
-  <si>
     <t>MaLoaiHinh</t>
   </si>
   <si>
     <t>TenLoaiHinh</t>
   </si>
   <si>
-    <t>MaTT</t>
-  </si>
-  <si>
-    <t>TenTT</t>
-  </si>
-  <si>
     <t>MaTTDH</t>
   </si>
   <si>
-    <t>MaTTDH (constraint)</t>
-  </si>
-  <si>
-    <t>DiaChiCH</t>
-  </si>
-  <si>
-    <t>MaDH (unique)</t>
+    <t>ChiTietMatHang</t>
+  </si>
+  <si>
+    <t>TenCL</t>
+  </si>
+  <si>
+    <t>ThoiGianDatHang</t>
+  </si>
+  <si>
+    <t>ChiTietTinhTrangDonHang</t>
+  </si>
+  <si>
+    <t>CuaHang</t>
+  </si>
+  <si>
+    <t>MaCH</t>
+  </si>
+  <si>
+    <t>ThoiGianTaoHoaDon</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -612,6 +603,20 @@
       <u/>
       <sz val="11"/>
       <color theme="4" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="5"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -725,7 +730,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -844,18 +849,26 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1636,8 +1649,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B1:R52"/>
   <sheetViews>
-    <sheetView topLeftCell="I1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Q13" sqref="Q13"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L30" sqref="L30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2430,34 +2443,36 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35F3918C-7D5D-45E4-A643-8C85C44C52CF}">
-  <dimension ref="D3:T13"/>
+  <dimension ref="C3:R14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="N23" sqref="N23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="3" max="3" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.140625" customWidth="1"/>
-    <col min="6" max="6" width="15.42578125" customWidth="1"/>
-    <col min="7" max="7" width="12.140625" customWidth="1"/>
-    <col min="8" max="8" width="13.85546875" customWidth="1"/>
-    <col min="9" max="9" width="13.5703125" customWidth="1"/>
-    <col min="10" max="10" width="15" customWidth="1"/>
-    <col min="11" max="11" width="12" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="22.7109375" customWidth="1"/>
-    <col min="13" max="13" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="17.85546875" customWidth="1"/>
-    <col min="15" max="15" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="18.28515625" customWidth="1"/>
-    <col min="18" max="18" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="7.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="4:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="C3" s="2" t="s">
+        <v>158</v>
+      </c>
       <c r="D3" s="2" t="s">
         <v>3</v>
       </c>
@@ -2465,52 +2480,49 @@
         <v>1</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>156</v>
+        <v>5</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>157</v>
+        <v>9</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>8</v>
+        <v>130</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>159</v>
+        <v>10</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>130</v>
+        <v>12</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>10</v>
+        <v>161</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="O3" s="2" t="s">
-        <v>12</v>
+        <v>162</v>
       </c>
       <c r="P3" s="2" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="Q3" s="2" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="R3" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="S3" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="T3" s="2" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="4" spans="4:20" x14ac:dyDescent="0.25">
+    <row r="4" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="C4" s="46" t="s">
+        <v>2</v>
+      </c>
       <c r="D4" s="35" t="s">
         <v>56</v>
       </c>
@@ -2521,320 +2533,307 @@
         <v>149</v>
       </c>
       <c r="G4" s="35" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="H4" s="35" t="s">
         <v>152</v>
       </c>
       <c r="I4" s="35" t="s">
-        <v>152</v>
+        <v>11</v>
       </c>
       <c r="J4" s="35" t="s">
-        <v>153</v>
+        <v>11</v>
       </c>
       <c r="K4" s="35" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="L4" s="35" t="s">
-        <v>11</v>
-      </c>
-      <c r="M4" s="35" t="s">
-        <v>11</v>
+        <v>14</v>
+      </c>
+      <c r="M4" s="46" t="s">
+        <v>157</v>
       </c>
       <c r="N4" s="35" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="O4" s="35" t="s">
-        <v>14</v>
+        <v>163</v>
       </c>
       <c r="P4" s="35" t="s">
-        <v>164</v>
+        <v>40</v>
       </c>
       <c r="Q4" s="35" t="s">
-        <v>162</v>
+        <v>45</v>
       </c>
       <c r="R4" s="35" t="s">
-        <v>40</v>
-      </c>
-      <c r="S4" s="35" t="s">
-        <v>45</v>
-      </c>
-      <c r="T4" s="35" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="5" spans="4:20" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="C5" s="46" t="s">
+        <v>149</v>
+      </c>
       <c r="D5" s="36" t="s">
         <v>57</v>
       </c>
       <c r="E5" s="36" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="35" t="s">
+      <c r="F5" s="36" t="s">
+        <v>150</v>
+      </c>
+      <c r="G5" s="36" t="s">
+        <v>153</v>
+      </c>
+      <c r="H5" s="36" t="s">
+        <v>159</v>
+      </c>
+      <c r="I5" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="G5" s="36" t="s">
-        <v>150</v>
-      </c>
-      <c r="H5" s="35" t="s">
-        <v>2</v>
-      </c>
-      <c r="I5" s="36" t="s">
-        <v>154</v>
-      </c>
-      <c r="J5" s="35" t="s">
-        <v>2</v>
+      <c r="J5" s="36" t="s">
+        <v>15</v>
       </c>
       <c r="K5" s="36" t="s">
-        <v>155</v>
-      </c>
-      <c r="L5" s="35" t="s">
-        <v>2</v>
-      </c>
-      <c r="M5" s="36" t="s">
-        <v>15</v>
+        <v>156</v>
+      </c>
+      <c r="L5" s="36" t="s">
+        <v>13</v>
+      </c>
+      <c r="M5" s="46" t="s">
+        <v>11</v>
       </c>
       <c r="N5" s="36" t="s">
-        <v>161</v>
-      </c>
-      <c r="O5" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="P5" s="36" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q5" s="43" t="s">
+        <v>27</v>
+      </c>
+      <c r="O5" s="43" t="s">
+        <v>38</v>
+      </c>
+      <c r="P5" s="34" t="s">
         <v>163</v>
       </c>
-      <c r="R5" s="45" t="s">
-        <v>38</v>
-      </c>
-      <c r="S5" s="36" t="s">
+      <c r="Q5" s="36" t="s">
         <v>42</v>
       </c>
-      <c r="T5" s="36" t="s">
+      <c r="R5" s="36" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="6" spans="4:20" x14ac:dyDescent="0.25">
+    <row r="6" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="C6" s="46" t="s">
+        <v>151</v>
+      </c>
       <c r="D6" s="36"/>
       <c r="E6" s="36" t="s">
         <v>6</v>
       </c>
       <c r="F6" s="36" t="s">
+        <v>27</v>
+      </c>
+      <c r="G6" s="36" t="s">
+        <v>27</v>
+      </c>
+      <c r="H6" s="36" t="s">
+        <v>27</v>
+      </c>
+      <c r="I6" s="36" t="s">
         <v>131</v>
       </c>
-      <c r="G6" s="36" t="s">
-        <v>151</v>
-      </c>
-      <c r="H6" s="36" t="s">
-        <v>131</v>
-      </c>
-      <c r="I6" s="36" t="s">
-        <v>151</v>
-      </c>
       <c r="J6" s="36" t="s">
-        <v>131</v>
+        <v>16</v>
       </c>
       <c r="K6" s="36" t="s">
-        <v>151</v>
+        <v>27</v>
       </c>
       <c r="L6" s="36" t="s">
-        <v>131</v>
+        <v>23</v>
       </c>
       <c r="M6" s="36" t="s">
-        <v>16</v>
-      </c>
-      <c r="N6" s="36"/>
-      <c r="O6" s="36" t="s">
+        <v>36</v>
+      </c>
+      <c r="N6" s="39"/>
+      <c r="O6" s="45" t="s">
         <v>23</v>
       </c>
       <c r="P6" s="34" t="s">
-        <v>162</v>
-      </c>
-      <c r="Q6" s="36"/>
-      <c r="R6" s="36" t="s">
-        <v>166</v>
-      </c>
-      <c r="S6" s="36" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q6" s="36" t="s">
         <v>24</v>
       </c>
-      <c r="T6" s="36"/>
-    </row>
-    <row r="7" spans="4:20" x14ac:dyDescent="0.25">
+      <c r="R6" s="36"/>
+    </row>
+    <row r="7" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="C7" s="46" t="s">
+        <v>152</v>
+      </c>
       <c r="D7" s="36"/>
       <c r="E7" s="36" t="s">
         <v>7</v>
       </c>
-      <c r="F7" s="36" t="s">
-        <v>158</v>
-      </c>
-      <c r="G7" s="34"/>
-      <c r="H7" s="36" t="s">
-        <v>158</v>
-      </c>
+      <c r="F7" s="34"/>
+      <c r="G7" s="36"/>
+      <c r="H7" s="36"/>
       <c r="I7" s="36"/>
       <c r="J7" s="36" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="K7" s="36"/>
-      <c r="L7" s="36"/>
-      <c r="M7" s="36" t="s">
-        <v>18</v>
-      </c>
-      <c r="N7" s="36"/>
-      <c r="O7" s="36" t="s">
+      <c r="L7" s="36" t="s">
+        <v>24</v>
+      </c>
+      <c r="M7" s="34" t="s">
+        <v>45</v>
+      </c>
+      <c r="N7" s="39"/>
+      <c r="O7" s="48" t="s">
         <v>24</v>
       </c>
       <c r="P7" s="34" t="s">
         <v>45</v>
       </c>
-      <c r="Q7" s="36"/>
-      <c r="R7" s="46" t="s">
-        <v>24</v>
-      </c>
-      <c r="S7" s="36" t="s">
+      <c r="Q7" s="36" t="s">
         <v>25</v>
       </c>
-      <c r="T7" s="36"/>
-    </row>
-    <row r="8" spans="4:20" x14ac:dyDescent="0.25">
+      <c r="R7" s="36"/>
+    </row>
+    <row r="8" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="C8" s="36" t="s">
+        <v>6</v>
+      </c>
       <c r="D8" s="36"/>
       <c r="E8" s="34" t="s">
         <v>56</v>
       </c>
-      <c r="F8" s="34"/>
+      <c r="F8" s="36"/>
       <c r="G8" s="36"/>
       <c r="H8" s="36"/>
       <c r="I8" s="36"/>
-      <c r="J8" s="36"/>
+      <c r="J8" s="36" t="s">
+        <v>19</v>
+      </c>
       <c r="K8" s="36"/>
-      <c r="L8" s="36"/>
-      <c r="M8" s="36" t="s">
-        <v>19</v>
-      </c>
-      <c r="N8" s="36"/>
-      <c r="O8" s="36" t="s">
+      <c r="L8" s="36" t="s">
         <v>25</v>
       </c>
-      <c r="Q8" s="36"/>
-      <c r="R8" s="36" t="s">
-        <v>41</v>
-      </c>
-      <c r="S8" s="36" t="s">
+      <c r="M8" s="36"/>
+      <c r="N8" s="39"/>
+      <c r="O8" s="39"/>
+      <c r="P8" s="36" t="s">
+        <v>164</v>
+      </c>
+      <c r="Q8" s="36" t="s">
         <v>23</v>
       </c>
-      <c r="T8" s="36"/>
-    </row>
-    <row r="9" spans="4:20" x14ac:dyDescent="0.25">
+      <c r="R8" s="36"/>
+    </row>
+    <row r="9" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="C9" s="36" t="s">
+        <v>7</v>
+      </c>
       <c r="D9" s="36"/>
       <c r="E9" s="38"/>
-      <c r="F9" s="38"/>
+      <c r="F9" s="36"/>
       <c r="G9" s="36"/>
       <c r="H9" s="36"/>
       <c r="I9" s="36"/>
-      <c r="J9" s="36"/>
+      <c r="J9" s="36" t="s">
+        <v>20</v>
+      </c>
       <c r="K9" s="36"/>
       <c r="L9" s="36"/>
-      <c r="M9" s="36" t="s">
-        <v>20</v>
-      </c>
+      <c r="M9" s="36"/>
       <c r="N9" s="36"/>
       <c r="O9" s="36"/>
-      <c r="P9" s="36"/>
-      <c r="Q9" s="36"/>
-      <c r="R9" s="36" t="s">
-        <v>42</v>
-      </c>
-      <c r="S9" s="34" t="s">
+      <c r="P9" s="39"/>
+      <c r="Q9" s="37" t="s">
         <v>58</v>
       </c>
-      <c r="T9" s="36"/>
-    </row>
-    <row r="10" spans="4:20" x14ac:dyDescent="0.25">
+      <c r="R9" s="36"/>
+    </row>
+    <row r="10" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="C10" s="44" t="s">
+        <v>131</v>
+      </c>
       <c r="D10" s="36"/>
       <c r="E10" s="39"/>
-      <c r="F10" s="42"/>
-      <c r="G10" s="41"/>
-      <c r="H10" s="41"/>
+      <c r="F10" s="41"/>
+      <c r="G10" s="36"/>
+      <c r="H10" s="36"/>
       <c r="I10" s="36"/>
-      <c r="J10" s="36"/>
+      <c r="J10" s="36" t="s">
+        <v>21</v>
+      </c>
       <c r="K10" s="36"/>
       <c r="L10" s="36"/>
-      <c r="M10" s="36" t="s">
-        <v>21</v>
-      </c>
+      <c r="M10" s="36"/>
       <c r="N10" s="36"/>
       <c r="O10" s="36"/>
-      <c r="P10" s="36"/>
-      <c r="Q10" s="36"/>
-      <c r="R10" s="34" t="s">
-        <v>167</v>
-      </c>
-      <c r="T10" s="36"/>
-    </row>
-    <row r="11" spans="4:20" x14ac:dyDescent="0.25">
+      <c r="P10" s="39"/>
+      <c r="R10" s="36"/>
+    </row>
+    <row r="11" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="C11" s="45" t="s">
+        <v>154</v>
+      </c>
       <c r="D11" s="36"/>
       <c r="E11" s="39"/>
-      <c r="F11" s="42"/>
+      <c r="F11" s="37"/>
       <c r="G11" s="37"/>
       <c r="H11" s="37"/>
       <c r="I11" s="37"/>
-      <c r="J11" s="37"/>
-      <c r="K11" s="37"/>
-      <c r="L11" s="37"/>
-      <c r="M11" s="34" t="s">
-        <v>160</v>
-      </c>
+      <c r="J11" s="34" t="s">
+        <v>155</v>
+      </c>
+      <c r="K11" s="36"/>
+      <c r="L11" s="36"/>
+      <c r="M11" s="36"/>
       <c r="N11" s="36"/>
       <c r="O11" s="36"/>
       <c r="P11" s="36"/>
-      <c r="Q11" s="36"/>
+      <c r="Q11" s="41"/>
       <c r="R11" s="36"/>
-      <c r="S11" s="36"/>
-      <c r="T11" s="36"/>
-    </row>
-    <row r="12" spans="4:20" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="C12" s="39"/>
       <c r="D12" s="36"/>
       <c r="E12" s="39"/>
-      <c r="F12" s="39"/>
+      <c r="F12" s="40"/>
       <c r="G12" s="40"/>
       <c r="H12" s="40"/>
       <c r="I12" s="40"/>
-      <c r="J12" s="40"/>
-      <c r="K12" s="40"/>
-      <c r="L12" s="40"/>
-      <c r="M12" s="34" t="s">
+      <c r="J12" s="34" t="s">
         <v>14</v>
       </c>
+      <c r="K12" s="36"/>
+      <c r="L12" s="36"/>
+      <c r="M12" s="36"/>
       <c r="N12" s="36"/>
       <c r="O12" s="36"/>
       <c r="P12" s="36"/>
       <c r="Q12" s="36"/>
       <c r="R12" s="36"/>
-      <c r="S12" s="36"/>
-      <c r="T12" s="36"/>
-    </row>
-    <row r="13" spans="4:20" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="C13" s="39"/>
       <c r="D13" s="36"/>
       <c r="E13" s="36"/>
       <c r="F13" s="36"/>
       <c r="G13" s="36"/>
       <c r="H13" s="36"/>
       <c r="I13" s="36"/>
-      <c r="J13" s="36"/>
-      <c r="K13" s="36"/>
+      <c r="J13" s="42"/>
+      <c r="K13" s="34"/>
       <c r="L13" s="36"/>
-      <c r="M13" s="44" t="s">
-        <v>165</v>
-      </c>
-      <c r="N13" s="34"/>
+      <c r="M13" s="36"/>
+      <c r="N13" s="36"/>
       <c r="O13" s="36"/>
       <c r="P13" s="36"/>
       <c r="Q13" s="36"/>
       <c r="R13" s="36"/>
-      <c r="S13" s="36"/>
-      <c r="T13" s="36"/>
+    </row>
+    <row r="14" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="J14" s="47"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>